<commit_message>
Buying vehicles Controllers updated
The program now saves information from the carmodel only. It also breaks when the information is read from the file... May need to redo the reading and writing from binary file.
</commit_message>
<xml_diff>
--- a/CarModelTables.xlsx
+++ b/CarModelTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giuseppe\Desktop\Project For C++\C-ManagementApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E81E49C9-E549-4D09-9A87-6DB39BE77207}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A45E2-64A9-4263-9E62-65E657CE7ABC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15060" windowHeight="5115" xr2:uid="{5FF6CDEF-1D15-4129-AA7D-2BE0CB28B241}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Make</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Date-Sold</t>
-  </si>
-  <si>
-    <t>Extras</t>
   </si>
   <si>
     <t>Author</t>
@@ -546,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B689162-04F5-459F-806A-69E48296C366}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,9 +566,9 @@
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -580,12 +577,12 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -593,9 +590,9 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>43204</v>
@@ -606,7 +603,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>
@@ -615,9 +612,9 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="2"/>
@@ -626,9 +623,9 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -639,120 +636,84 @@
       <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1001</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D7" s="4">
         <v>2006</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="4">
-        <v>6</v>
-      </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1002</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="D8" s="4">
         <v>1994</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="4">
-        <v>5.7</v>
-      </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1003</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="4">
         <v>2013</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="4">
-        <v>2.5</v>
-      </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1004</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D10" s="4">
         <v>2007</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="4">
-        <v>6.1</v>
-      </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1005</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D11" s="4">
         <v>2007</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="4">
-        <v>5</v>
-      </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -761,7 +722,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -770,9 +731,9 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="2"/>
@@ -781,9 +742,9 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
@@ -791,25 +752,32 @@
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2"/>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1001</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="4">
+        <v>6</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
@@ -818,13 +786,17 @@
         <v>1002</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="4">
+        <v>5.7</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
@@ -833,13 +805,17 @@
         <v>1003</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2.5</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
@@ -848,13 +824,17 @@
         <v>1004</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="4">
+        <v>6.1</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
@@ -863,13 +843,17 @@
         <v>1005</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="4">
+        <v>5</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
@@ -893,7 +877,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="2"/>
@@ -904,10 +888,10 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>8</v>
@@ -1000,7 +984,7 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="2"/>
@@ -1011,22 +995,22 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="G33" s="2"/>
     </row>

</xml_diff>

<commit_message>
Revert "Buying vehicles Controllers updated"
This reverts commit 48d3cc76dd695129ee1525e081133501df131a62.
</commit_message>
<xml_diff>
--- a/CarModelTables.xlsx
+++ b/CarModelTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giuseppe\Desktop\Project For C++\C-ManagementApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A45E2-64A9-4263-9E62-65E657CE7ABC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E81E49C9-E549-4D09-9A87-6DB39BE77207}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15060" windowHeight="5115" xr2:uid="{5FF6CDEF-1D15-4129-AA7D-2BE0CB28B241}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Make</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Date-Sold</t>
+  </si>
+  <si>
+    <t>Extras</t>
   </si>
   <si>
     <t>Author</t>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B689162-04F5-459F-806A-69E48296C366}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,9 +569,9 @@
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -577,12 +580,12 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -590,9 +593,9 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>43204</v>
@@ -603,7 +606,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>
@@ -612,9 +615,9 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="2"/>
@@ -623,9 +626,9 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -636,84 +639,120 @@
       <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1001</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4">
         <v>2006</v>
       </c>
+      <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="4">
+        <v>6</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1002</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="4">
         <v>1994</v>
       </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5.7</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1003</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="4">
         <v>2013</v>
       </c>
+      <c r="E9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2.5</v>
+      </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1004</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="4">
         <v>2007</v>
       </c>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="4">
+        <v>6.1</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1005</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4">
         <v>2007</v>
       </c>
+      <c r="E11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -722,7 +761,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -731,9 +770,9 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="2"/>
@@ -742,9 +781,9 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
@@ -752,32 +791,25 @@
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1001</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="4">
-        <v>6</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
@@ -786,17 +818,13 @@
         <v>1002</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="4">
-        <v>5.7</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
@@ -805,17 +833,13 @@
         <v>1003</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="4">
-        <v>2.5</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
@@ -824,17 +848,13 @@
         <v>1004</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="4">
-        <v>6.1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
@@ -843,17 +863,13 @@
         <v>1005</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="4">
-        <v>5</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
@@ -877,7 +893,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="2"/>
@@ -888,10 +904,10 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>8</v>
@@ -984,7 +1000,7 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="2"/>
@@ -995,22 +1011,22 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G33" s="2"/>
     </row>

</xml_diff>